<commit_message>
README updated, added interface description generation, renamed loopback to logical
</commit_message>
<xml_diff>
--- a/config/source/config_db.xlsx
+++ b/config/source/config_db.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/messg/WorkDocs/Study/Networking/MPLS In SDN Era/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/messg/WorkDocs/Study/Networking/MPLS In SDN Era/Config_generator/config/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23651EB1-5D19-E845-9A1B-372962F562D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE97A0BF-B80C-5B42-B459-2C0337964812}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20640" yWindow="-28800" windowWidth="34360" windowHeight="28800" activeTab="2" xr2:uid="{E82CC42B-01EB-FF47-9CF2-3579C257240A}"/>
+    <workbookView xWindow="-20640" yWindow="-28340" windowWidth="34360" windowHeight="28340" activeTab="1" xr2:uid="{E82CC42B-01EB-FF47-9CF2-3579C257240A}"/>
   </bookViews>
   <sheets>
     <sheet name="physical_interfaces" sheetId="1" r:id="rId1"/>
     <sheet name="loopback_interfaces" sheetId="2" r:id="rId2"/>
     <sheet name="devices" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -164,9 +164,6 @@
     <t>192.168.10.1</t>
   </si>
   <si>
-    <t>lo0.0</t>
-  </si>
-  <si>
     <t>192.168.10.2</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>192.168.20.4</t>
+  </si>
+  <si>
+    <t>lo0</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="str">
-        <f>_xlfn.CONCAT(E4,"_",F4,":",I4,"_",H4)</f>
+        <f t="shared" ref="B4:B20" si="0">_xlfn.CONCAT(E4,"_",F4,":",I4,"_",H4)</f>
         <v>CE1_xe-0/0/2:xe-0/0/1_PE1</v>
       </c>
       <c r="C4" t="s">
@@ -620,13 +620,13 @@
         <v>12</v>
       </c>
       <c r="J4">
-        <f>SUM(G4,1)</f>
+        <f t="shared" ref="J4:J20" si="1">SUM(G4,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="str">
-        <f>_xlfn.CONCAT(E5,"_",F5,":",I5,"_",H5)</f>
+        <f t="shared" si="0"/>
         <v>CE1_xe-0/0/3:xe-0/0/1_PE2</v>
       </c>
       <c r="C5" t="s">
@@ -651,13 +651,13 @@
         <v>12</v>
       </c>
       <c r="J5">
-        <f>SUM(G5,1)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="str">
-        <f>_xlfn.CONCAT(E6,"_",F6,":",I6,"_",H6)</f>
+        <f t="shared" si="0"/>
         <v>CE2_xe-0/0/2:xe-0/0/2_PE1</v>
       </c>
       <c r="C6" t="s">
@@ -682,13 +682,13 @@
         <v>13</v>
       </c>
       <c r="J6">
-        <f>SUM(G6,1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="str">
-        <f>_xlfn.CONCAT(E7,"_",F7,":",I7,"_",H7)</f>
+        <f t="shared" si="0"/>
         <v>CE2_xe-0/0/3:xe-0/0/0_PE2</v>
       </c>
       <c r="C7" t="s">
@@ -713,13 +713,13 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <f>SUM(G7,1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="str">
-        <f>_xlfn.CONCAT(E8,"_",F8,":",I8,"_",H8)</f>
+        <f t="shared" si="0"/>
         <v>PE1_xe-0/0/3:xe-0/0/2_PE2</v>
       </c>
       <c r="C8" t="s">
@@ -744,13 +744,13 @@
         <v>13</v>
       </c>
       <c r="J8">
-        <f>SUM(G8,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="str">
-        <f>_xlfn.CONCAT(E9,"_",F9,":",I9,"_",H9)</f>
+        <f t="shared" si="0"/>
         <v>PE1_xe-0/0/4:xe-0/0/1_P1</v>
       </c>
       <c r="C9" t="s">
@@ -775,13 +775,13 @@
         <v>12</v>
       </c>
       <c r="J9">
-        <f>SUM(G9,1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" t="str">
-        <f>_xlfn.CONCAT(E10,"_",F10,":",I10,"_",H10)</f>
+        <f t="shared" si="0"/>
         <v>PE2_xe-0/0/3:xe-0/0/0_P2</v>
       </c>
       <c r="C10" t="s">
@@ -806,7 +806,7 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <f>SUM(G10,1)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="M10" t="s">
@@ -815,7 +815,7 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" t="str">
-        <f>_xlfn.CONCAT(E11,"_",F11,":",I11,"_",H11)</f>
+        <f t="shared" si="0"/>
         <v>P1_xe-0/0/3:xe-0/0/2_P2</v>
       </c>
       <c r="C11" t="s">
@@ -840,13 +840,13 @@
         <v>13</v>
       </c>
       <c r="J11">
-        <f>SUM(G11,1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="str">
-        <f>_xlfn.CONCAT(E12,"_",F12,":",I12,"_",H12)</f>
+        <f t="shared" si="0"/>
         <v>P1_xe-0/0/4:xe-0/0/3_P2</v>
       </c>
       <c r="C12" t="s">
@@ -871,13 +871,13 @@
         <v>15</v>
       </c>
       <c r="J12">
-        <f>SUM(G12,1)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="str">
-        <f>_xlfn.CONCAT(E13,"_",F13,":",I13,"_",H13)</f>
+        <f t="shared" si="0"/>
         <v>P1_xe-0/0/2:xe-0/0/1_RR1</v>
       </c>
       <c r="C13" t="s">
@@ -902,13 +902,13 @@
         <v>12</v>
       </c>
       <c r="J13">
-        <f>SUM(G13,1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="str">
-        <f>_xlfn.CONCAT(E14,"_",F14,":",I14,"_",H14)</f>
+        <f t="shared" si="0"/>
         <v>P2_xe-0/0/1:xe-0/0/3_RR1</v>
       </c>
       <c r="C14" t="s">
@@ -933,13 +933,13 @@
         <v>15</v>
       </c>
       <c r="J14">
-        <f>SUM(G14,1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" t="str">
-        <f>_xlfn.CONCAT(E15,"_",F15,":",I15,"_",H15)</f>
+        <f t="shared" si="0"/>
         <v>RR1_xe-0/0/2:xe-0/0/1_RR2</v>
       </c>
       <c r="C15" t="s">
@@ -964,13 +964,13 @@
         <v>12</v>
       </c>
       <c r="J15">
-        <f>SUM(G15,1)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="str">
-        <f>_xlfn.CONCAT(E16,"_",F16,":",I16,"_",H16)</f>
+        <f t="shared" si="0"/>
         <v>P1_xe-0/0/6:xe-0/0/1_PE3</v>
       </c>
       <c r="C16" t="s">
@@ -995,13 +995,13 @@
         <v>12</v>
       </c>
       <c r="J16">
-        <f>SUM(G16,1)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" t="str">
-        <f>_xlfn.CONCAT(E17,"_",F17,":",I17,"_",H17)</f>
+        <f t="shared" si="0"/>
         <v>P1_xe-0/0/5:xe-0/0/0_RR2</v>
       </c>
       <c r="C17" t="s">
@@ -1026,13 +1026,13 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <f>SUM(G17,1)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" t="str">
-        <f>_xlfn.CONCAT(E18,"_",F18,":",I18,"_",H18)</f>
+        <f t="shared" si="0"/>
         <v>P2_xe-0/0/4:xe-0/0/2_RR2</v>
       </c>
       <c r="C18" t="s">
@@ -1057,13 +1057,13 @@
         <v>13</v>
       </c>
       <c r="J18">
-        <f>SUM(G18,1)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" t="str">
-        <f>_xlfn.CONCAT(E19,"_",F19,":",I19,"_",H19)</f>
+        <f t="shared" si="0"/>
         <v>P2_xe-0/0/5:xe-0/0/0_PE4</v>
       </c>
       <c r="C19" t="s">
@@ -1088,13 +1088,13 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <f>SUM(G19,1)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" t="str">
-        <f>_xlfn.CONCAT(E20,"_",F20,":",I20,"_",H20)</f>
+        <f t="shared" si="0"/>
         <v>PE3_xe-0/0/2:xe-0/0/1_PE4</v>
       </c>
       <c r="C20" t="s">
@@ -1119,7 +1119,7 @@
         <v>12</v>
       </c>
       <c r="J20">
-        <f>SUM(G20,1)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" t="str">
-        <f t="shared" ref="B31:B40" si="0">_xlfn.CONCAT(E31,"_",F31,":",I31,"_",H31)</f>
+        <f t="shared" ref="B31:B37" si="2">_xlfn.CONCAT(E31,"_",F31,":",I31,"_",H31)</f>
         <v>PE3_xe-0/0/3:xe-0/0/0_BRS</v>
       </c>
       <c r="C31" t="s">
@@ -1253,7 +1253,7 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>PE4_xe-0/0/2:xe-0/0/1_BRS</v>
       </c>
       <c r="C32" t="s">
@@ -1283,7 +1283,7 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BR3_xe-0/0/1:xe-0/0/2_BRS</v>
       </c>
       <c r="C33" t="s">
@@ -1313,7 +1313,7 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BR4_xe-0/0/1:xe-0/0/3_BRS</v>
       </c>
       <c r="C34" t="s">
@@ -1343,7 +1343,7 @@
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BR3_xe-0/0/2:xe-0/0/1_H3S</v>
       </c>
       <c r="C35" t="s">
@@ -1373,7 +1373,7 @@
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BR4_xe-0/0/2:xe-0/0/2_H3S</v>
       </c>
       <c r="C36" t="s">
@@ -1403,7 +1403,7 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>H3_xe-0/0/1:xe-0/0/3_H3S</v>
       </c>
       <c r="C37" t="s">
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A294F2-8499-C840-8CD8-9FF748E9FD7B}">
   <dimension ref="B6:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1454,7 +1454,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
@@ -1465,10 +1465,10 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
         <v>43</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
@@ -1476,10 +1476,10 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
@@ -1487,10 +1487,10 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
@@ -1498,10 +1498,10 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
@@ -1509,10 +1509,10 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
@@ -1520,10 +1520,10 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
@@ -1531,10 +1531,10 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
@@ -1542,10 +1542,10 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
@@ -1553,10 +1553,10 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
@@ -1564,10 +1564,10 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -1575,10 +1575,10 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1590,7 +1590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778CA92D-E6C5-6B4D-8E83-69863952A720}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>